<commit_message>
change test.xl, extends num of sheets to 5
</commit_message>
<xml_diff>
--- a/myway/excel/test.xlsx
+++ b/myway/excel/test.xlsx
@@ -3,15 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="식당판매" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="매점판매" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="장의용품" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="상복" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="기타" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mg4b92lLJmHto8xbigvelFNMY59Mg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mjZxa6sqW0u2RTWGtMIwWTbN9l3Fw=="/>
     </ext>
   </extLst>
 </workbook>
@@ -235,6 +237,14 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -681,6 +691,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <pageSetUpPr/>
@@ -1955,7 +1993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <pageSetUpPr/>

</xml_diff>

<commit_message>
change test.xl, edit setlist()
</commit_message>
<xml_diff>
--- a/myway/excel/test.xlsx
+++ b/myway/excel/test.xlsx
@@ -13,45 +13,33 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mjZxa6sqW0u2RTWGtMIwWTbN9l3Fw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mhWYUTytX4QOE8ZLP5IQ3SELPDMHQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t>물품명</t>
   </si>
   <si>
-    <t>단위</t>
-  </si>
-  <si>
     <t>단가</t>
   </si>
   <si>
     <t>수량</t>
   </si>
   <si>
-    <t>금액</t>
-  </si>
-  <si>
     <t>고무장갑</t>
   </si>
   <si>
-    <t>개</t>
-  </si>
-  <si>
     <t>수세미</t>
   </si>
   <si>
     <t>녹차</t>
   </si>
   <si>
-    <t>통</t>
-  </si>
-  <si>
     <t>부의봉투</t>
   </si>
   <si>
@@ -73,48 +61,60 @@
     <t>종이컵</t>
   </si>
   <si>
-    <t>줄</t>
-  </si>
-  <si>
     <t>노트</t>
   </si>
   <si>
     <t>박스테잎</t>
   </si>
   <si>
+    <t>삼겹살</t>
+  </si>
+  <si>
+    <t>대패삼겹살</t>
+  </si>
+  <si>
+    <t>치즈김밥</t>
+  </si>
+  <si>
+    <t>김밥</t>
+  </si>
+  <si>
+    <t>닭볶음탕</t>
+  </si>
+  <si>
+    <t>콜라</t>
+  </si>
+  <si>
+    <t>사이다</t>
+  </si>
+  <si>
+    <t>주스</t>
+  </si>
+  <si>
+    <t>맥주</t>
+  </si>
+  <si>
+    <t>소주</t>
+  </si>
+  <si>
+    <t>신라면(컵)</t>
+  </si>
+  <si>
+    <t>육개장(컵)</t>
+  </si>
+  <si>
+    <t>밥공기(1)</t>
+  </si>
+  <si>
+    <t>접시180(1)</t>
+  </si>
+  <si>
+    <t>식탁보</t>
+  </si>
+  <si>
     <t>부의금가방</t>
   </si>
   <si>
-    <t>신라면(컵)</t>
-  </si>
-  <si>
-    <t>육개장(컵)</t>
-  </si>
-  <si>
-    <t>밥공기(1)</t>
-  </si>
-  <si>
-    <t>접시180(1)</t>
-  </si>
-  <si>
-    <t>식탁보</t>
-  </si>
-  <si>
-    <t>콜라</t>
-  </si>
-  <si>
-    <t>사이다</t>
-  </si>
-  <si>
-    <t>주스</t>
-  </si>
-  <si>
-    <t>맥주</t>
-  </si>
-  <si>
-    <t>소주</t>
-  </si>
-  <si>
     <t>양주</t>
   </si>
   <si>
@@ -140,21 +140,6 @@
   </si>
   <si>
     <t>된장국</t>
-  </si>
-  <si>
-    <t>삼겹살</t>
-  </si>
-  <si>
-    <t>대패삼겹살</t>
-  </si>
-  <si>
-    <t>치즈김밥</t>
-  </si>
-  <si>
-    <t>김밥</t>
-  </si>
-  <si>
-    <t>닭볶음탕</t>
   </si>
   <si>
     <t>치킨</t>
@@ -204,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -214,11 +199,14 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,228 +450,116 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
         <v>2300.0</v>
       </c>
-      <c r="D2" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="1">
-        <f t="shared" ref="E2:E13" si="1">D2*C2</f>
-        <v>0</v>
-      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
         <v>1000.0</v>
       </c>
-      <c r="D3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
         <v>3300.0</v>
       </c>
-      <c r="D4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1">
+      <c r="B5" s="1">
         <v>800.0</v>
       </c>
-      <c r="D5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
         <v>780.0</v>
       </c>
-      <c r="D6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C6" s="3">
+        <v>3.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
         <v>1100.0</v>
       </c>
-      <c r="D7" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
         <v>1000.0</v>
       </c>
-      <c r="D8" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
         <v>1000.0</v>
       </c>
-      <c r="D9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
         <v>2600.0</v>
       </c>
-      <c r="D10" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="1">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
         <v>1500.0</v>
       </c>
-      <c r="D11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
         <v>600.0</v>
       </c>
-      <c r="D12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
         <v>1600.0</v>
       </c>
-      <c r="D13" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C13" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -699,7 +575,84 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1100.0</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1000.0</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3000.0</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2500.0</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1">
+        <v>9000.0</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -713,7 +666,99 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1000.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1000.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1200.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4">
+        <v>4000.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4000.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="4">
+        <v>930.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1050.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4">
+        <v>6000.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1200.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="4">
+        <v>6000.0</v>
+      </c>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -728,276 +773,136 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="22" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="4">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4">
+        <v>930.0</v>
+      </c>
+    </row>
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1050.0</v>
+      </c>
+    </row>
+    <row r="5" ht="13.5" customHeight="1">
+      <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4">
+        <v>6000.0</v>
+      </c>
+    </row>
+    <row r="6" ht="13.5" customHeight="1">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1200.0</v>
+      </c>
+    </row>
+    <row r="7" ht="13.5" customHeight="1">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6000.0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="8" ht="13.5" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="3">
-        <v>5000.0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="3">
-        <f t="shared" ref="E2:E15" si="1">D2*C2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="B8" s="4">
+        <v>1000.0</v>
+      </c>
+    </row>
+    <row r="9" ht="13.5" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3">
-        <v>930.0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="B9" s="4">
+        <v>1000.0</v>
+      </c>
+    </row>
+    <row r="10" ht="13.5" customHeight="1">
+      <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1050.0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="B10" s="4">
+        <v>1200.0</v>
+      </c>
+    </row>
+    <row r="11" ht="13.5" customHeight="1">
+      <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3">
-        <v>6000.0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="B11" s="4">
+        <v>4000.0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="12" ht="13.5" customHeight="1">
+      <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1200.0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3">
-        <v>6000.0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1000.0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1000.0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1200.0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E10" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="B12" s="4">
         <v>4000.0</v>
       </c>
-      <c r="D11" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E11" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3">
-        <v>4000.0</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="B13" s="4">
         <v>12000.0</v>
       </c>
-      <c r="D13" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="B14" s="4">
         <v>12000.0</v>
       </c>
-      <c r="D14" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E14" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3">
+      <c r="B15" s="4">
         <v>8000.0</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1"/>
@@ -1975,16 +1880,6 @@
     <row r="988" ht="13.5" customHeight="1"/>
     <row r="989" ht="13.5" customHeight="1"/>
     <row r="990" ht="13.5" customHeight="1"/>
-    <row r="991" ht="13.5" customHeight="1"/>
-    <row r="992" ht="13.5" customHeight="1"/>
-    <row r="993" ht="13.5" customHeight="1"/>
-    <row r="994" ht="13.5" customHeight="1"/>
-    <row r="995" ht="13.5" customHeight="1"/>
-    <row r="996" ht="13.5" customHeight="1"/>
-    <row r="997" ht="13.5" customHeight="1"/>
-    <row r="998" ht="13.5" customHeight="1"/>
-    <row r="999" ht="13.5" customHeight="1"/>
-    <row r="1000" ht="13.5" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -2003,258 +1898,161 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="22" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="1">
         <v>8000.0</v>
       </c>
-      <c r="D2" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="1">
-        <f t="shared" ref="E2:E14" si="1">D2*C2</f>
-        <v>0</v>
+      <c r="C2" s="3">
+        <v>3.0</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B3" s="1">
         <v>8000.0</v>
       </c>
-      <c r="D3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C3" s="3">
+        <v>2.0</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B4" s="1">
         <v>2400.0</v>
       </c>
-      <c r="D4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C4" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B5" s="1">
         <v>2600.0</v>
       </c>
-      <c r="D5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C5" s="3">
+        <v>4.0</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6" s="1">
         <v>2600.0</v>
       </c>
-      <c r="D6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C6" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B7" s="1">
         <v>3000.0</v>
       </c>
-      <c r="D7" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C7" s="3">
+        <v>23.0</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1">
         <v>3000.0</v>
       </c>
-      <c r="D8" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C8" s="3">
+        <v>65.0</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1">
         <v>2000.0</v>
       </c>
-      <c r="D9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C9" s="3">
+        <v>43.0</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1">
         <v>2500.0</v>
       </c>
-      <c r="D10" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C10" s="3">
+        <v>234.0</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1">
         <v>2000.0</v>
       </c>
-      <c r="D11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C11" s="3">
+        <v>44.0</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1">
         <v>9000.0</v>
       </c>
-      <c r="D12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C12" s="3">
+        <v>23.0</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1">
         <v>8000.0</v>
       </c>
-      <c r="D13" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C13" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="1">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1">
         <v>9000.0</v>
       </c>
-      <c r="D14" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C14" s="3">
+        <v>43.0</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1"/>
@@ -3234,15 +3032,6 @@
     <row r="989" ht="13.5" customHeight="1"/>
     <row r="990" ht="13.5" customHeight="1"/>
     <row r="991" ht="13.5" customHeight="1"/>
-    <row r="992" ht="13.5" customHeight="1"/>
-    <row r="993" ht="13.5" customHeight="1"/>
-    <row r="994" ht="13.5" customHeight="1"/>
-    <row r="995" ht="13.5" customHeight="1"/>
-    <row r="996" ht="13.5" customHeight="1"/>
-    <row r="997" ht="13.5" customHeight="1"/>
-    <row r="998" ht="13.5" customHeight="1"/>
-    <row r="999" ht="13.5" customHeight="1"/>
-    <row r="1000" ht="13.5" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>